<commit_message>
feat(data): update demo data
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="series" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t xml:space="preserve">titulo</t>
   </si>
@@ -103,6 +103,9 @@
     <t xml:space="preserve">Descripción Episodio 2 Serie 1</t>
   </si>
   <si>
+    <t xml:space="preserve">https://cdn.coverr.co/videos/coverr-a-beautiful-domestic-cat-with-green-eyes-4785/1080p.mp4</t>
+  </si>
+  <si>
     <t xml:space="preserve">serie-1_episodio-2.jpg</t>
   </si>
   <si>
@@ -306,10 +309,16 @@
     <t xml:space="preserve">serie-2_episodio-5.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Serie 1</t>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serie-1_showcase.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Descripción Serie 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serie-2_showcase.jpg</t>
   </si>
 </sst>
 </file>
@@ -478,8 +487,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,10 +554,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,19 +565,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,19 +585,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,19 +605,19 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,19 +625,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,19 +645,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,19 +665,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,19 +685,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,19 +705,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -729,11 +738,14 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.07"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -751,7 +763,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,7 +774,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(data): update sample data
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="series" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="temporadas" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="episodios" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="showcase" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,104 +21,116 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+  <si>
+    <t xml:space="preserve">id_temporada</t>
+  </si>
   <si>
     <t xml:space="preserve">titulo</t>
   </si>
   <si>
-    <t xml:space="preserve">descripcion_completa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">descripcion_corta</t>
+    <t xml:space="preserve">descripcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preview_img_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temproada_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporada 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Temporada 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporada_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporada 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Temporada 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporada_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporada 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Temporada 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titulo_serie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titulo_episodio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video_url</t>
   </si>
   <si>
     <t xml:space="preserve">Serie 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Compĺeta Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Corta Serie 1</t>
+    <t xml:space="preserve">Título Episodio 1 (Serie 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 1 Serie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://test-videos.co.uk/vids/bigbuckbunny/mp4/h264/720/Big_Buck_Bunny_720_10s_2MB.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serie-1_episodio-1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título Episodio 2 (Serie 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 2 Serie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn.coverr.co/videos/coverr-a-beautiful-domestic-cat-with-green-eyes-4785/1080p.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serie-1_episodio-2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título Episodio 3 (Serie 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 3 Serie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serie-1_episodio-3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título Episodio 4 (Serie 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 4 Serie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serie-1_episodio-4.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título Episodio 5 (Serie 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 5 Serie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serie-1_episodio-5.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Serie 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Compĺeta Serie 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Corta Serie 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">titulo_serie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">titulo_episodio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">descripcion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">video_url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preview_img_url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 1 (Serie 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 1 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://test-videos.co.uk/vids/bigbuckbunny/mp4/h264/720/Big_Buck_Bunny_720_10s_2MB.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 2 (Serie 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 2 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cdn.coverr.co/videos/coverr-a-beautiful-domestic-cat-with-green-eyes-4785/1080p.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 3 (Serie 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 3 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-3.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 4 (Serie 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 4 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-4.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 5 (Serie 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 5 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-5.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Título Episodio 1 (Serie 2)</t>
   </si>
   <si>
@@ -163,18 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">serie-2_episodio-5.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_showcase.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Serie 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-2_showcase.jpg</t>
   </si>
 </sst>
 </file>
@@ -275,55 +274,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -338,8 +350,8 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,281 +365,221 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.07"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(data/source): update data source
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t xml:space="preserve">id_temporada</t>
   </si>
@@ -44,6 +44,9 @@
     <t xml:space="preserve">Descripción Temporada 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Temporada_1.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Temporada_2</t>
   </si>
   <si>
@@ -53,16 +56,16 @@
     <t xml:space="preserve">Descripción Temporada 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Temporada_2.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Temporada_3</t>
   </si>
   <si>
     <t xml:space="preserve">Temporada 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Temporada 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">titulo_serie</t>
+    <t xml:space="preserve">id_episodio</t>
   </si>
   <si>
     <t xml:space="preserve">titulo_episodio</t>
@@ -74,106 +77,82 @@
     <t xml:space="preserve">video_url</t>
   </si>
   <si>
-    <t xml:space="preserve">Serie 1</t>
+    <t xml:space="preserve">episodio-1_temporada-1</t>
   </si>
   <si>
     <t xml:space="preserve">Título Episodio 1 (Serie 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Episodio 1 Serie 1</t>
+    <t xml:space="preserve">Descripción Episodio 1 Temporada 1</t>
   </si>
   <si>
     <t xml:space="preserve">https://test-videos.co.uk/vids/bigbuckbunny/mp4/h264/720/Big_Buck_Bunny_720_10s_2MB.mp4</t>
   </si>
   <si>
-    <t xml:space="preserve">serie-1_episodio-1.jpg</t>
+    <t xml:space="preserve">Episodio-1_Temporada-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-2_temporada-1</t>
   </si>
   <si>
     <t xml:space="preserve">Título Episodio 2 (Serie 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Episodio 2 Serie 1</t>
+    <t xml:space="preserve">Descripción Episodio 2 Temporada 1</t>
   </si>
   <si>
     <t xml:space="preserve">https://cdn.coverr.co/videos/coverr-a-beautiful-domestic-cat-with-green-eyes-4785/1080p.mp4</t>
   </si>
   <si>
-    <t xml:space="preserve">serie-1_episodio-2.jpg</t>
+    <t xml:space="preserve">Episodio-2_Temporada-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-3_temporada-1</t>
   </si>
   <si>
     <t xml:space="preserve">Título Episodio 3 (Serie 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Episodio 3 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-3.jpg</t>
+    <t xml:space="preserve">Descripción Episodio 3 Temporada 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episodio-3_Temporada-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-1_temporada-2</t>
   </si>
   <si>
     <t xml:space="preserve">Título Episodio 4 (Serie 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Episodio 4 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-4.jpg</t>
+    <t xml:space="preserve">Descripción Episodio 1 Temporada 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episodio-1_Temporada-2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-2_temporada-2</t>
   </si>
   <si>
     <t xml:space="preserve">Título Episodio 5 (Serie 1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Episodio 5 Serie 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-1_episodio-5.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serie 2</t>
+    <t xml:space="preserve">Descripción Episodio 2 Temporada 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episodio-2_Temporada-2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-3_temporada-2</t>
   </si>
   <si>
     <t xml:space="preserve">Título Episodio 1 (Serie 2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción Episodio 1 Serie 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-2_episodio-1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 2 (Serie 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 2 Serie 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-2_episodio-2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 3 (Serie 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 3 Serie 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-2_episodio-3.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 4 (Serie 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 4 Serie 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-2_episodio-4.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título Episodio 5 (Serie 2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descripción Episodio 5 Serie 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serie-2_episodio-5.jpg</t>
+    <t xml:space="preserve">Descripción Episodio 3 Temporada 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episodio-3_Temporada-2.png</t>
   </si>
 </sst>
 </file>
@@ -183,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -204,6 +183,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -248,12 +232,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,62 +262,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -348,53 +345,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="78.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="81.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
+      <c r="A1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
+      <c r="A2" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>20</v>
@@ -402,186 +403,144 @@
       <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
+      <c r="A3" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
+      <c r="A4" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
+      <c r="A5" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
+      <c r="A6" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
+      <c r="A7" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A8" s="0"/>
+      <c r="C8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A9" s="0"/>
+      <c r="C9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A10" s="0"/>
+      <c r="C10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="A11" s="0"/>
+      <c r="C11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat(data): updat edata source
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t xml:space="preserve">id_temporada</t>
   </si>
@@ -83,6 +83,9 @@
     <t xml:space="preserve">duracion</t>
   </si>
   <si>
+    <t xml:space="preserve">portada</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-1_temporada-1</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
     <t xml:space="preserve">1h 35min</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-1_Temporada-1_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-2_temporada-1</t>
   </si>
   <si>
@@ -116,6 +122,9 @@
     <t xml:space="preserve">Episodio-2_Temporada-1.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-2_Temporada-1_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-3_temporada-1</t>
   </si>
   <si>
@@ -131,6 +140,9 @@
     <t xml:space="preserve">50min</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-3_Temporada-1_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-1_temporada-2</t>
   </si>
   <si>
@@ -146,6 +158,9 @@
     <t xml:space="preserve">1h 25min</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-1_Temporada-2_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-2_temporada-2</t>
   </si>
   <si>
@@ -158,6 +173,9 @@
     <t xml:space="preserve">Episodio-2_Temporada-2.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-2_Temporada-2_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-3_temporada-2</t>
   </si>
   <si>
@@ -170,6 +188,9 @@
     <t xml:space="preserve">Episodio-3_Temporada-2.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-3_Temporada-2_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-1_temporada-3</t>
   </si>
   <si>
@@ -182,6 +203,9 @@
     <t xml:space="preserve">Episodio-1_Temporada-3.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-1_Temporada-3_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-2_temporada-3</t>
   </si>
   <si>
@@ -194,6 +218,9 @@
     <t xml:space="preserve">Episodio-2_Temporada-3.png</t>
   </si>
   <si>
+    <t xml:space="preserve">Episodio-2_Temporada-3_Portada.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-3_temporada-3</t>
   </si>
   <si>
@@ -204,6 +231,9 @@
   </si>
   <si>
     <t xml:space="preserve">Episodio-3_Temporada-3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episodio-3_Temporada-3_Portada.png</t>
   </si>
 </sst>
 </file>
@@ -391,10 +421,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -436,266 +466,296 @@
       <c r="I1" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>2023</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>2023</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>2023</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat(data): update data source
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -341,7 +341,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="1" sqref="E:E F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,7 +432,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="81.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.04"/>

</xml_diff>

<commit_message>
chore: udpate data source
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t xml:space="preserve">id_temporada</t>
   </si>
@@ -104,9 +104,6 @@
     <t xml:space="preserve">1h 35min</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-1_Temporada-1_Portada.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">episodio-2_temporada-1</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t xml:space="preserve">Episodio-2_Temporada-1.png</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-2_Temporada-1_Portada.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">episodio-3_temporada-1</t>
   </si>
   <si>
@@ -140,7 +134,7 @@
     <t xml:space="preserve">50min</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-3_Temporada-1_Portada.png</t>
+    <t xml:space="preserve">Temporada_3.png</t>
   </si>
   <si>
     <t xml:space="preserve">episodio-1_temporada-2</t>
@@ -158,9 +152,6 @@
     <t xml:space="preserve">1h 25min</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-1_Temporada-2_Portada.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">episodio-2_temporada-2</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t xml:space="preserve">Episodio-2_Temporada-2.png</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-2_Temporada-2_Portada.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">episodio-3_temporada-2</t>
   </si>
   <si>
@@ -188,9 +176,6 @@
     <t xml:space="preserve">Episodio-3_Temporada-2.png</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-3_Temporada-2_Portada.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">episodio-1_temporada-3</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
     <t xml:space="preserve">Episodio-1_Temporada-3.png</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-1_Temporada-3_Portada.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">episodio-2_temporada-3</t>
   </si>
   <si>
@@ -218,9 +200,6 @@
     <t xml:space="preserve">Episodio-2_Temporada-3.png</t>
   </si>
   <si>
-    <t xml:space="preserve">Episodio-2_Temporada-3_Portada.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">episodio-3_temporada-3</t>
   </si>
   <si>
@@ -231,17 +210,15 @@
   </si>
   <si>
     <t xml:space="preserve">Episodio-3_Temporada-3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Episodio-3_Temporada-3_Portada.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -308,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,6 +295,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,7 +322,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="1" sqref="E:E F16"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="J10 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,7 +405,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E:E"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,7 +413,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="81.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.04"/>
@@ -498,31 +479,31 @@
       <c r="I2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>27</v>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>2022</v>
@@ -530,95 +511,95 @@
       <c r="I3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>33</v>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>2022</v>
@@ -626,95 +607,95 @@
       <c r="I6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>50</v>
+      <c r="J6" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>2023</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>60</v>
+        <v>42</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>2023</v>
@@ -722,31 +703,31 @@
       <c r="I9" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="0" t="s">
-        <v>65</v>
+      <c r="J9" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>2023</v>
@@ -754,8 +735,8 @@
       <c r="I10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>70</v>
+      <c r="J10" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
feat(data): udpate data source
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
     <t xml:space="preserve">id_temporada</t>
   </si>
@@ -137,6 +137,15 @@
     <t xml:space="preserve">Temporada_3.png</t>
   </si>
   <si>
+    <t xml:space="preserve">episodio-4_temporada-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título Episodio 4 (Temporada 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 4 Temporada 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-1_temporada-2</t>
   </si>
   <si>
@@ -176,6 +185,15 @@
     <t xml:space="preserve">Episodio-3_Temporada-2.png</t>
   </si>
   <si>
+    <t xml:space="preserve">episodio-4_temporada-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título Episodio 4 (Temporada 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 4 Temporada 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-1_temporada-3</t>
   </si>
   <si>
@@ -210,6 +228,15 @@
   </si>
   <si>
     <t xml:space="preserve">Episodio-3_Temporada-3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-4_temporada-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Título Episodio 4 (Temporada 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descripción Episodio 4 Temporada 3</t>
   </si>
 </sst>
 </file>
@@ -322,7 +349,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="J10 E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -402,10 +429,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -552,13 +579,13 @@
         <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>40</v>
@@ -567,180 +594,289 @@
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>2022</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>2022</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="1"/>
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat(lib/components): impl iframe video player
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t xml:space="preserve">id_temporada</t>
   </si>
@@ -77,40 +77,43 @@
     <t xml:space="preserve">La mayoría de las autoridades reguladoras, como la FDA o la EMA, consideran que la "supervivencia global" y la "supervivencia. En este capítulo explicaremos cada uno de estos conceptos. libre de progresión" son unos de los criterios más importantes para aprobar un nuevo tratamiento o indicación.</t>
   </si>
   <si>
+    <t xml:space="preserve">https://mydrive.merck.com/personal/etorre12_merck_com/_layouts/15/embed.aspx?UniqueId=b16f7933-2fb5-4fde-9712-4ddd8c718711&amp;embed=%7B%22ust%22%3Atrue%2C%22hv%22%3A%22CopyEmbedCode%22%7D&amp;referrer=StreamWebApp&amp;referrerScenario=EmbedDialog.Create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episodio-1_Temporada-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h 35min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-2_temporada-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RECIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En este capítulo vamos a hablar de cómo se evalúa la respuesta al tratamiento del cáncer. Siempre que los oncólogos se refieren a la capacidad de un tratamiento para reducir un tumor, utilizan criterios estandarizados internacionalmente. Estos criterios se denominan: Criterios de Evaluación de Respuesta en Tumores Sólidos o criterios RECIST, por sus siglas en inglés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn.coverr.co/videos/coverr-a-beautiful-domestic-cat-with-green-eyes-4785/1080p.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episodio-2_Temporada-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temporada_2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">episodio-3_temporada-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervivencia en Enfermedad Temprana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La evaluación del tiempo en que un cáncer permanece bajo control es una de las variables más importantes en oncología. Existen diferentes tipos de supervivencia, en este capítulo describiremos algunos de los más conocidos (RFS, DFS, EFS).</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://test-videos.co.uk/vids/bigbuckbunny/mp4/h264/720/Big_Buck_Bunny_720_10s_2MB.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Episodio-1_Temporada-1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1h 35min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">episodio-2_temporada-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RECIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En este capítulo vamos a hablar de cómo se evalúa la respuesta al tratamiento del cáncer. Siempre que los oncólogos se refieren a la capacidad de un tratamiento para reducir un tumor, utilizan criterios estandarizados internacionalmente. Estos criterios se denominan: Criterios de Evaluación de Respuesta en Tumores Sólidos o criterios RECIST, por sus siglas en inglés.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://cdn.coverr.co/videos/coverr-a-beautiful-domestic-cat-with-green-eyes-4785/1080p.mp4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Episodio-2_Temporada-1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temporada_2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">episodio-3_temporada-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supervivencia en Enfermedad Temprana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La evaluación del tiempo en que un cáncer permanece bajo control es una de las variables más importantes en oncología. Existen diferentes tipos de supervivencia, en este capítulo describiremos algunos de los más conocidos (RFS, DFS, EFS).</t>
   </si>
   <si>
     <t xml:space="preserve">Episodio-3_Temporada-1.png</t>
@@ -154,7 +157,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,6 +178,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,12 +229,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,7 +335,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,10 +397,10 @@
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="1" t="n">
@@ -412,7 +426,7 @@
       <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -427,7 +441,7 @@
       <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -448,48 +462,48 @@
         <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>2025</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>2026</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>7</v>
@@ -497,31 +511,31 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>2027</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>7</v>
@@ -533,16 +547,14 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="0"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="0"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H10" s="1"/>
@@ -552,7 +564,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="3"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H13" s="1"/>
@@ -570,6 +582,9 @@
       <c r="J15" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://mydrive.merck.com/personal/etorre12_merck_com/_layouts/15/embed.aspx?UniqueId=b16f7933-2fb5-4fde-9712-4ddd8c718711&amp;embed=%7B%22ust%22%3Atrue%2C%22hv%22%3A%22CopyEmbedCode%22%7D&amp;referrer=StreamWebApp&amp;referrerScenario=EmbedDialog.Create"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
chore: update dummy database
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t xml:space="preserve">id_temporada</t>
   </si>
@@ -68,6 +68,9 @@
     <t xml:space="preserve">portada</t>
   </si>
   <si>
+    <t xml:space="preserve">proximamente</t>
+  </si>
+  <si>
     <t xml:space="preserve">trailer-1_temporada-1</t>
   </si>
   <si>
@@ -86,15 +89,16 @@
     <t xml:space="preserve">https://images.pexels.com/photos/5726788/pexels-photo-5726788.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">episodio-1_temporada-1</t>
   </si>
   <si>
     <t xml:space="preserve">Supervivencia</t>
   </si>
   <si>
-    <t xml:space="preserve">La mayoría de las autoridades reguladoras, como la FDA o la EMA, consideran que la "supervivencia global" y la "supervivencia libre de progresión" son unos de los criterios más importantes para aprobar un nuevo tratamiento o indicación.
-En este capítulo explicaremos cada uno de estos conceptos.
-</t>
+    <t xml:space="preserve">La mayoría de las autoridades reguladoras, como la FDA o la EMA, consideran que la "supervivencia global" y la "supervivencia libre de progresión" son unos de los criterios más importantes para aprobar un nuevo tratamiento o indicación. En este capítulo explicaremos cada uno de estos conceptos.</t>
   </si>
   <si>
     <t xml:space="preserve">https://mydrive.merck.com/personal/etorre12_merck_com/_layouts/15/embed.aspx?UniqueId=d457f53c-c243-40c5-aae5-5df337754cef&amp;embed=%7B%22hvm%22%3Atrue%2C%22ust%22%3Atrue%7D&amp;referrer=OneUpFileViewer&amp;referrerScenario=EmbedDialog.Create</t>
@@ -140,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">Temporada_2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si</t>
   </si>
   <si>
     <t xml:space="preserve">episodio-3_temporada-1</t>
@@ -408,7 +415,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="C5 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,10 +467,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,6 +482,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="81.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,208 +516,246 @@
       <c r="J1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>2023</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>2023</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>2024</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>2025</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>2026</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K6" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>2027</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K7" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J9" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="5"/>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://collaboration.merck.com/sites/onconceptos/_layouts/15/embed.aspx?UniqueId=3934dfb1-e42b-4782-8a02-093fbd8326a6&amp;embed=%7B%22hvm%22%3Atrue%2C%22ust%22%3Atrue%7D&amp;referrer=OneUpFileViewer&amp;referrerScenario=EmbedDialog.Create"/>

</xml_diff>

<commit_message>
chore: update dummy db
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -164,7 +164,7 @@
     <t xml:space="preserve">Temporada_3.png</t>
   </si>
   <si>
-    <t xml:space="preserve">9/jun/2023</t>
+    <t xml:space="preserve">5/jul/2023</t>
   </si>
   <si>
     <t xml:space="preserve">episodio-4_temporada-1</t>
@@ -223,11 +223,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -273,12 +274,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -325,8 +320,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,7 +353,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -442,331 +441,331 @@
   </sheetPr>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="44.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="N2" s="1" t="n">
+      <c r="M2" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N2" s="2" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="N3" s="1" t="n">
+      <c r="M3" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="M4" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="N4" s="8" t="n">
+      <c r="N4" s="9" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="2" t="n">
         <v>2025</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="N5" s="1" t="n">
+      <c r="M5" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N5" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="2" t="n">
         <v>2026</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="N6" s="1" t="n">
+      <c r="M6" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N6" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="2" t="n">
         <v>2027</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="N7" s="1" t="n">
+      <c r="M7" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N7" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -802,36 +801,36 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="n">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: udpate dummy db
</commit_message>
<xml_diff>
--- a/public/datos-onconceptos.xlsx
+++ b/public/datos-onconceptos.xlsx
@@ -113,7 +113,7 @@
     <t xml:space="preserve">https://images.pexels.com/photos/5965598/pexels-photo-5965598.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
   </si>
   <si>
-    <t xml:space="preserve">7/jun/2023</t>
+    <t xml:space="preserve">23/jun/2023</t>
   </si>
   <si>
     <t xml:space="preserve">https://forms.office.com/Pages/ResponsePage.aspx?id=7OQNoKhIpkO-dOMSdOIGDQBVwII28rdEjX_x9IJb6lhUMVlKUkpDWjZGTEhRMkU0T0wySVNRSVBTMSQlQCNjPTEu</t>
@@ -441,8 +441,8 @@
   </sheetPr>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -584,10 +584,10 @@
         <v>30</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>31</v>

</xml_diff>